<commit_message>
Made mode for months + days, got time to sync with PC on compile
</commit_message>
<xml_diff>
--- a/Count Up Box Features.xlsx
+++ b/Count Up Box Features.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Feature</t>
   </si>
@@ -25,9 +25,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Decimals on all time units</t>
-  </si>
-  <si>
     <t>Scroll through units with rotary</t>
   </si>
   <si>
@@ -47,6 +44,12 @@
   </si>
   <si>
     <t>Days constrained by month</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Properly display time with 0s</t>
   </si>
 </sst>
 </file>
@@ -391,7 +394,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,42 +416,54 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>